<commit_message>
Added police dispatch call view page
</commit_message>
<xml_diff>
--- a/Data/MPD Communications Codes.xlsx
+++ b/Data/MPD Communications Codes.xlsx
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>